<commit_message>
Updated Excel Files from atlas-data as of 2024-03-11
</commit_message>
<xml_diff>
--- a/public/excel-files/atlas-tactics.xlsx
+++ b/public/excel-files/atlas-tactics.xlsx
@@ -79,46 +79,46 @@
     <t>AML.TA0003</t>
   </si>
   <si>
-    <t>x-mitre-tactic--169cdf3d-886b-4d3e-a26d-11a848920ea8</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--da8d1d9d-c45d-4d56-8874-d7cd5886dc25</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--e67a0f3d-a541-401f-801e-e62a9fdeca70</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--e81ccab1-e5f8-4d4f-be66-24dbe74fe5db</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--95274328-9e38-4bdd-9d2e-0e80e1256ff0</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--02d1fc74-a19e-406f-9ecc-df96a8d18856</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--7b38d743-e6b2-4a99-a497-bbc97db9a761</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--57175629-3f53-4980-a99d-8725df069f91</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--cf90e8f7-7829-431f-866f-66e6dd9e18a2</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--d4010b82-406a-46ba-83a1-23c16db77604</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--714edce4-f9ef-4b9a-b0ae-56e70a3cb15c</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--4acc5de3-5a7c-4ac8-8e7f-0e9f25e7e725</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--c79e43f1-2a18-48d4-af61-40091b1f1a37</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--90786da6-b4a6-4741-9bab-a87fdf42a05b</t>
+    <t>x-mitre-tactic--b88656b8-92b5-48c8-aa0d-401d09225c3a</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--8407dd06-d298-4fcb-b42c-5e459685d96c</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--aea8785b-aff2-4ffb-97a9-724e16802cd0</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--38834033-1aaf-4fac-a120-baae566da1f4</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--560abc82-7f87-4ae5-8d5a-18e0de351c4e</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--86985fad-fc0c-4b01-9441-f1c005dc529e</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--f84385a0-14f1-41d0-8256-02e34d3b6fd1</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--332194a6-2b0b-445e-900f-28c5588d3996</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--eec9cdf5-d82d-4b12-8d7c-5bcf661c4c8c</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--7343b749-f8e5-4bc5-88a3-78b80a05456c</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--a2b28f78-92b9-476f-968c-427462a3d057</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--d7e6e3f1-7033-47a0-b162-51cffda7932a</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--0bdff1ba-04fb-43bc-9559-de278508fe94</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--d59655a1-d955-47af-bea8-a776ae7383bb</t>
   </si>
   <si>
     <t>Collection</t>
@@ -198,7 +198,7 @@
   <si>
     <t xml:space="preserve">The adversary is trying to steal machine learning artifacts or other information about the machine learning system.
 Exfiltration consists of techniques that adversaries may use to steal data from your network.
-Data may be stolen for it's valuable intellectual property, or for use in staging future operations.
+Data may be stolen for its valuable intellectual property, or for use in staging future operations.
 Techniques for getting data out of a target network typically include transferring it over their command and control channel or an alternate channel and may also include putting size limits on the transmission.
 </t>
   </si>
@@ -307,7 +307,7 @@
     <t>https://atlas.mitre.org/tactics/AML.TA0003</t>
   </si>
   <si>
-    <t>31 October 2023</t>
+    <t>11 March 2024</t>
   </si>
 </sst>
 </file>

</xml_diff>